<commit_message>
Changed Return of AmbulanceMap to be ServerResponse in relevant parts
</commit_message>
<xml_diff>
--- a/amo/hexCodes/Ambulance_Map.xlsx
+++ b/amo/hexCodes/Ambulance_Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrkh\Desktop\YelloCo\5.Fifth Task\AMSServices\amo\hexCodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C850A10E-01B4-4C5F-BE5D-0828EC8B5621}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CA70AB-E5B7-4C8E-AAD3-A56AB57216DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Code</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>Old entry to be used for history</t>
+  </si>
+  <si>
+    <t>Insert Ambulance Map</t>
+  </si>
+  <si>
+    <t>Insertion Successful</t>
+  </si>
+  <si>
+    <t>Failed To insert because the car already has resources assigned</t>
+  </si>
+  <si>
+    <t>Failed to insert because car is already assigned elsewhere</t>
+  </si>
+  <si>
+    <t>Delete Ambulance Map</t>
+  </si>
+  <si>
+    <t>Deleted Successfully</t>
+  </si>
+  <si>
+    <t>Failed to delete</t>
   </si>
 </sst>
 </file>
@@ -58,12 +79,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,11 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,6 +443,58 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>